<commit_message>
New Features and update GitIgnoreList
</commit_message>
<xml_diff>
--- a/doc/sit_afast.xlsx
+++ b/doc/sit_afast.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\naldodj-DataSul2TotvsProtheus\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\naldodj-DataSul2TotvsProtheus\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3187" uniqueCount="207">
   <si>
     <t>datasul</t>
   </si>
@@ -560,9 +560,6 @@
     <t>N    NN                                                                                          SS</t>
   </si>
   <si>
-    <t>DATASUL</t>
-  </si>
-  <si>
     <t>03</t>
   </si>
   <si>
@@ -636,6 +633,15 @@
   </si>
   <si>
     <t>001</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Datasul</t>
+  </si>
+  <si>
+    <t>Protheus</t>
   </si>
 </sst>
 </file>
@@ -17281,9 +17287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E81"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17296,10 +17300,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
+        <v>205</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -17307,13 +17320,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -17325,13 +17338,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -17343,13 +17356,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -17361,13 +17374,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -17379,13 +17392,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -17397,13 +17410,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -17415,13 +17428,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -17433,13 +17446,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -17451,13 +17464,13 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -17469,13 +17482,13 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C11" s="4">
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
@@ -17487,13 +17500,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
@@ -17505,13 +17518,13 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
@@ -17523,10 +17536,10 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
@@ -17538,13 +17551,13 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E15" t="s">
         <v>49</v>
@@ -17556,10 +17569,10 @@
         <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E16" t="s">
         <v>53</v>
@@ -17570,10 +17583,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E17" t="s">
         <v>55</v>
@@ -17584,10 +17597,10 @@
         <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E18" t="s">
         <v>58</v>
@@ -17598,13 +17611,13 @@
         <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="4">
         <v>30</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
         <v>59</v>
@@ -17615,13 +17628,13 @@
         <v>44</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -17632,10 +17645,10 @@
         <v>45</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E21" t="s">
         <v>62</v>
@@ -17646,13 +17659,13 @@
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -17663,13 +17676,13 @@
         <v>47</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E23" t="s">
         <v>65</v>
@@ -17680,13 +17693,13 @@
         <v>48</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E24" t="s">
         <v>67</v>
@@ -17697,13 +17710,13 @@
         <v>49</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="4">
         <v>30</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E25" t="s">
         <v>68</v>
@@ -17714,10 +17727,10 @@
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E26" t="s">
         <v>70</v>
@@ -17728,13 +17741,13 @@
         <v>51</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E27" t="s">
         <v>71</v>
@@ -17745,13 +17758,13 @@
         <v>52</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E28" t="s">
         <v>72</v>
@@ -17762,10 +17775,10 @@
         <v>53</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E29" t="s">
         <v>73</v>
@@ -17776,10 +17789,10 @@
         <v>54</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E30" t="s">
         <v>74</v>
@@ -17790,13 +17803,13 @@
         <v>55</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E31" t="s">
         <v>76</v>
@@ -17807,13 +17820,13 @@
         <v>56</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E32" t="s">
         <v>78</v>
@@ -17824,13 +17837,13 @@
         <v>57</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E33" t="s">
         <v>79</v>
@@ -17841,13 +17854,13 @@
         <v>58</v>
       </c>
       <c r="B34" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E34" t="s">
         <v>81</v>
@@ -17858,10 +17871,10 @@
         <v>59</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E35" t="s">
         <v>82</v>
@@ -17872,10 +17885,10 @@
         <v>60</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E36" t="s">
         <v>84</v>
@@ -17886,10 +17899,10 @@
         <v>61</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E37" t="s">
         <v>85</v>
@@ -17900,10 +17913,10 @@
         <v>62</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E38" t="s">
         <v>86</v>
@@ -17914,10 +17927,10 @@
         <v>63</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E39" t="s">
         <v>87</v>
@@ -17928,13 +17941,13 @@
         <v>64</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E40" t="s">
         <v>88</v>
@@ -17945,13 +17958,13 @@
         <v>65</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E41" t="s">
         <v>89</v>
@@ -17962,10 +17975,10 @@
         <v>66</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E42" t="s">
         <v>91</v>
@@ -17976,13 +17989,13 @@
         <v>67</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E43" t="s">
         <v>93</v>
@@ -17993,10 +18006,10 @@
         <v>68</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E44" t="s">
         <v>94</v>
@@ -18007,13 +18020,13 @@
         <v>69</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E45" t="s">
         <v>95</v>
@@ -18024,13 +18037,13 @@
         <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E46" t="s">
         <v>97</v>
@@ -18041,13 +18054,13 @@
         <v>71</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E47" t="s">
         <v>98</v>
@@ -18058,13 +18071,13 @@
         <v>72</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E48" t="s">
         <v>99</v>
@@ -18075,13 +18088,13 @@
         <v>73</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E49" t="s">
         <v>101</v>
@@ -18092,13 +18105,13 @@
         <v>74</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E50" t="s">
         <v>102</v>
@@ -18109,13 +18122,13 @@
         <v>77</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E51" t="s">
         <v>74</v>
@@ -18126,13 +18139,13 @@
         <v>78</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E52" t="s">
         <v>103</v>
@@ -18143,13 +18156,13 @@
         <v>79</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E53" t="s">
         <v>104</v>
@@ -18160,10 +18173,10 @@
         <v>80</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E54" t="s">
         <v>107</v>
@@ -18174,10 +18187,10 @@
         <v>81</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E55" t="s">
         <v>110</v>
@@ -18188,10 +18201,10 @@
         <v>82</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E56" t="s">
         <v>114</v>
@@ -18202,10 +18215,10 @@
         <v>83</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E57" t="s">
         <v>117</v>
@@ -18216,10 +18229,10 @@
         <v>84</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E58" t="s">
         <v>121</v>
@@ -18230,10 +18243,10 @@
         <v>85</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E59" t="s">
         <v>125</v>
@@ -18244,10 +18257,10 @@
         <v>86</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E60" t="s">
         <v>128</v>
@@ -18258,10 +18271,10 @@
         <v>87</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E61" t="s">
         <v>131</v>
@@ -18272,10 +18285,10 @@
         <v>88</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E62" t="s">
         <v>135</v>
@@ -18286,10 +18299,10 @@
         <v>89</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E63" t="s">
         <v>138</v>
@@ -18300,13 +18313,13 @@
         <v>90</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C64" s="4">
         <v>15</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E64" t="s">
         <v>141</v>
@@ -18317,10 +18330,10 @@
         <v>91</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E65" t="s">
         <v>144</v>
@@ -18331,10 +18344,10 @@
         <v>92</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E66" t="s">
         <v>62</v>
@@ -18345,13 +18358,13 @@
         <v>93</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E67" t="s">
         <v>149</v>
@@ -18362,13 +18375,13 @@
         <v>94</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E68" t="s">
         <v>152</v>
@@ -18379,10 +18392,10 @@
         <v>95</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E69" t="s">
         <v>153</v>
@@ -18393,13 +18406,13 @@
         <v>96</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E70" t="s">
         <v>155</v>
@@ -18410,13 +18423,13 @@
         <v>97</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E71" t="s">
         <v>157</v>
@@ -18427,13 +18440,13 @@
         <v>98</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E72" t="s">
         <v>158</v>
@@ -18444,10 +18457,10 @@
         <v>99</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E73" t="s">
         <v>162</v>
@@ -18458,10 +18471,10 @@
         <v>100</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E74" t="s">
         <v>165</v>
@@ -18472,13 +18485,13 @@
         <v>105</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E75" t="s">
         <v>167</v>
@@ -18489,10 +18502,10 @@
         <v>106</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E76" t="s">
         <v>169</v>
@@ -18503,10 +18516,10 @@
         <v>107</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E77" t="s">
         <v>172</v>
@@ -18517,10 +18530,10 @@
         <v>108</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E78" t="s">
         <v>173</v>
@@ -18531,10 +18544,10 @@
         <v>109</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E79" t="s">
         <v>173</v>
@@ -18545,10 +18558,10 @@
         <v>110</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E80" t="s">
         <v>176</v>
@@ -18559,10 +18572,10 @@
         <v>111</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E81" t="s">
         <v>172</v>
@@ -18578,8 +18591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18593,10 +18606,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -18604,13 +18626,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -18622,13 +18644,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -18640,13 +18662,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -18658,13 +18680,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -18676,13 +18698,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -18694,13 +18716,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -18712,13 +18734,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -18730,13 +18752,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -18748,13 +18770,13 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -18766,13 +18788,13 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
@@ -18784,13 +18806,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
@@ -18802,13 +18824,13 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
@@ -18820,13 +18842,13 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
@@ -18838,13 +18860,13 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E15" t="s">
         <v>49</v>
@@ -18856,13 +18878,13 @@
         <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E16" t="s">
         <v>53</v>
@@ -18874,13 +18896,13 @@
         <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E17" t="s">
         <v>55</v>
@@ -18891,13 +18913,13 @@
         <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E18" t="s">
         <v>58</v>
@@ -18908,13 +18930,13 @@
         <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E19" t="s">
         <v>59</v>
@@ -18925,13 +18947,13 @@
         <v>44</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -18942,13 +18964,13 @@
         <v>45</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E21" t="s">
         <v>62</v>
@@ -18959,13 +18981,13 @@
         <v>46</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -18976,13 +18998,13 @@
         <v>47</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E23" t="s">
         <v>65</v>
@@ -18993,13 +19015,13 @@
         <v>48</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E24" t="s">
         <v>67</v>
@@ -19010,13 +19032,13 @@
         <v>49</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E25" t="s">
         <v>68</v>
@@ -19027,13 +19049,13 @@
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E26" t="s">
         <v>70</v>
@@ -19044,13 +19066,13 @@
         <v>51</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E27" t="s">
         <v>71</v>
@@ -19061,13 +19083,13 @@
         <v>52</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E28" t="s">
         <v>72</v>
@@ -19078,13 +19100,13 @@
         <v>53</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E29" t="s">
         <v>73</v>
@@ -19095,13 +19117,13 @@
         <v>54</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E30" t="s">
         <v>74</v>
@@ -19112,13 +19134,13 @@
         <v>55</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E31" t="s">
         <v>76</v>
@@ -19129,13 +19151,13 @@
         <v>56</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E32" t="s">
         <v>78</v>
@@ -19146,13 +19168,13 @@
         <v>57</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E33" t="s">
         <v>79</v>
@@ -19163,13 +19185,13 @@
         <v>58</v>
       </c>
       <c r="B34" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E34" t="s">
         <v>81</v>
@@ -19180,13 +19202,13 @@
         <v>59</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E35" t="s">
         <v>82</v>
@@ -19197,13 +19219,13 @@
         <v>60</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E36" t="s">
         <v>84</v>
@@ -19214,13 +19236,13 @@
         <v>61</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E37" t="s">
         <v>85</v>
@@ -19231,13 +19253,13 @@
         <v>62</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E38" t="s">
         <v>86</v>
@@ -19248,13 +19270,13 @@
         <v>63</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E39" t="s">
         <v>87</v>
@@ -19265,13 +19287,13 @@
         <v>64</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E40" t="s">
         <v>88</v>
@@ -19282,13 +19304,13 @@
         <v>65</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E41" t="s">
         <v>89</v>
@@ -19299,13 +19321,13 @@
         <v>66</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E42" t="s">
         <v>91</v>
@@ -19316,13 +19338,13 @@
         <v>67</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E43" t="s">
         <v>93</v>
@@ -19333,13 +19355,13 @@
         <v>68</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E44" t="s">
         <v>94</v>
@@ -19350,13 +19372,13 @@
         <v>69</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E45" t="s">
         <v>95</v>
@@ -19367,13 +19389,13 @@
         <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E46" t="s">
         <v>97</v>
@@ -19384,13 +19406,13 @@
         <v>71</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E47" t="s">
         <v>98</v>
@@ -19401,13 +19423,13 @@
         <v>72</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E48" t="s">
         <v>99</v>
@@ -19418,13 +19440,13 @@
         <v>73</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E49" t="s">
         <v>101</v>
@@ -19435,13 +19457,13 @@
         <v>74</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E50" t="s">
         <v>102</v>
@@ -19452,13 +19474,13 @@
         <v>77</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E51" t="s">
         <v>74</v>
@@ -19469,13 +19491,13 @@
         <v>78</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E52" t="s">
         <v>103</v>
@@ -19486,13 +19508,13 @@
         <v>79</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E53" t="s">
         <v>104</v>
@@ -19503,13 +19525,13 @@
         <v>80</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E54" t="s">
         <v>107</v>
@@ -19520,13 +19542,13 @@
         <v>81</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E55" t="s">
         <v>110</v>
@@ -19537,13 +19559,13 @@
         <v>82</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E56" t="s">
         <v>114</v>
@@ -19554,13 +19576,13 @@
         <v>83</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E57" t="s">
         <v>117</v>
@@ -19571,13 +19593,13 @@
         <v>84</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E58" t="s">
         <v>121</v>
@@ -19588,13 +19610,13 @@
         <v>85</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E59" t="s">
         <v>125</v>
@@ -19605,13 +19627,13 @@
         <v>86</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E60" t="s">
         <v>128</v>
@@ -19622,13 +19644,13 @@
         <v>87</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E61" t="s">
         <v>131</v>
@@ -19639,13 +19661,13 @@
         <v>88</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E62" t="s">
         <v>135</v>
@@ -19656,13 +19678,13 @@
         <v>89</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E63" t="s">
         <v>138</v>
@@ -19673,13 +19695,13 @@
         <v>90</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E64" t="s">
         <v>141</v>
@@ -19690,13 +19712,13 @@
         <v>91</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E65" t="s">
         <v>144</v>
@@ -19707,13 +19729,13 @@
         <v>92</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E66" t="s">
         <v>62</v>
@@ -19724,13 +19746,13 @@
         <v>93</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E67" t="s">
         <v>149</v>
@@ -19741,13 +19763,13 @@
         <v>94</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E68" t="s">
         <v>152</v>
@@ -19758,13 +19780,13 @@
         <v>95</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E69" t="s">
         <v>153</v>
@@ -19775,13 +19797,13 @@
         <v>96</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E70" t="s">
         <v>155</v>
@@ -19792,13 +19814,13 @@
         <v>97</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E71" t="s">
         <v>157</v>
@@ -19809,13 +19831,13 @@
         <v>98</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E72" t="s">
         <v>158</v>
@@ -19826,13 +19848,13 @@
         <v>99</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E73" t="s">
         <v>162</v>
@@ -19843,13 +19865,13 @@
         <v>100</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E74" t="s">
         <v>165</v>
@@ -19860,13 +19882,13 @@
         <v>105</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E75" t="s">
         <v>167</v>
@@ -19877,13 +19899,13 @@
         <v>106</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E76" t="s">
         <v>169</v>
@@ -19894,13 +19916,13 @@
         <v>107</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E77" t="s">
         <v>172</v>
@@ -19911,13 +19933,13 @@
         <v>108</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E78" t="s">
         <v>173</v>
@@ -19928,13 +19950,13 @@
         <v>109</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E79" t="s">
         <v>173</v>
@@ -19945,13 +19967,13 @@
         <v>110</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E80" t="s">
         <v>176</v>
@@ -19962,13 +19984,13 @@
         <v>111</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="E81" t="s">
         <v>172</v>

</xml_diff>